<commit_message>
-updated quantity-tables based on Marc's feedback
</commit_message>
<xml_diff>
--- a/data-raw/quantity-tables.xlsx
+++ b/data-raw/quantity-tables.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="154">
   <si>
     <t>table</t>
   </si>
@@ -472,6 +472,21 @@
   </si>
   <si>
     <t>is_internal</t>
+  </si>
+  <si>
+    <t>enum</t>
+  </si>
+  <si>
+    <t>appropriationtypeenum</t>
+  </si>
+  <si>
+    <t>contracttypeenum</t>
+  </si>
+  <si>
+    <t>phaseormilestoneenum</t>
+  </si>
+  <si>
+    <t>reportcycleenum</t>
   </si>
 </sst>
 </file>
@@ -522,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -531,13 +546,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,7 +840,7 @@
     <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -846,7 +854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -860,7 +868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -874,7 +882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -888,7 +896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -902,7 +910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -917,7 +925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
@@ -932,7 +940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -947,7 +955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -960,8 +968,9 @@
       <c r="D9" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -974,36 +983,81 @@
       <c r="D10" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
@@ -1118,36 +1172,6 @@
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1159,7 +1183,7 @@
   <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1168,13 +1192,13 @@
     <col min="2" max="2" width="40.33203125" customWidth="1"/>
     <col min="3" max="3" width="38.88671875" customWidth="1"/>
     <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="3"/>
+    <col min="5" max="5" width="10.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1200,7 +1224,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -1220,7 +1244,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -1240,7 +1264,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1254,13 +1278,14 @@
       <c r="E4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="5" t="b">
+      <c r="F4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1274,15 +1299,18 @@
       <c r="E5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="5" t="b">
+      <c r="F5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1296,13 +1324,14 @@
       <c r="E6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="5" t="b">
+      <c r="F6" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1316,13 +1345,14 @@
       <c r="E7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="5" t="b">
+      <c r="F7" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -1336,13 +1366,14 @@
       <c r="E8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="5" t="b">
+      <c r="F8" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1356,13 +1387,14 @@
       <c r="E9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="5" t="b">
+      <c r="F9" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1376,13 +1408,14 @@
       <c r="E10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="5" t="b">
+      <c r="F10" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -1396,13 +1429,14 @@
       <c r="E11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="5" t="b">
+      <c r="F11" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -1416,13 +1450,14 @@
       <c r="E12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="5" t="b">
+      <c r="F12" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1436,13 +1471,14 @@
       <c r="E13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="5" t="b">
+      <c r="F13" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
@@ -1456,13 +1492,14 @@
       <c r="E14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="5" t="b">
+      <c r="F14" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -1476,13 +1513,14 @@
       <c r="E15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="5" t="b">
+      <c r="F15" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
@@ -1496,13 +1534,14 @@
       <c r="E16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="5" t="b">
+      <c r="F16" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1516,13 +1555,14 @@
       <c r="E17" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="5" t="b">
+      <c r="F17" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
@@ -1536,13 +1576,14 @@
       <c r="E18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="5" t="b">
+      <c r="F18" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
@@ -1556,15 +1597,18 @@
       <c r="E19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="5" t="b">
+      <c r="F19" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
@@ -1578,13 +1622,14 @@
       <c r="E20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="5" t="b">
+      <c r="F20" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>11</v>
       </c>
@@ -1598,13 +1643,14 @@
       <c r="E21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F21" s="5" t="b">
+      <c r="F21" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>11</v>
       </c>
@@ -1618,13 +1664,14 @@
       <c r="E22" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F22" s="5" t="b">
+      <c r="F22" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G22" s="3"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
@@ -1638,13 +1685,14 @@
       <c r="E23" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="5" t="b">
+      <c r="F23" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G23" s="3"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>11</v>
       </c>
@@ -1658,13 +1706,14 @@
       <c r="E24" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F24" s="5" t="b">
+      <c r="F24" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G24" s="3"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>11</v>
       </c>
@@ -1678,15 +1727,18 @@
       <c r="E25" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="5" t="b">
+      <c r="F25" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>11</v>
       </c>
@@ -1700,13 +1752,14 @@
       <c r="E26" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F26" s="5" t="b">
+      <c r="F26" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G26" s="3"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>11</v>
       </c>
@@ -1720,13 +1773,14 @@
       <c r="E27" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F27" s="5" t="b">
+      <c r="F27" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G27" s="3"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
@@ -1740,13 +1794,14 @@
       <c r="E28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F28" s="5" t="b">
+      <c r="F28" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G28" s="3"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>11</v>
       </c>
@@ -1760,13 +1815,14 @@
       <c r="E29" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="5" t="b">
+      <c r="F29" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G29" s="3"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>11</v>
       </c>
@@ -1778,15 +1834,16 @@
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" s="5" t="b">
+        <v>66</v>
+      </c>
+      <c r="F30" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G30" s="3"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>11</v>
       </c>
@@ -1800,13 +1857,14 @@
       <c r="E31" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F31" s="5" t="b">
+      <c r="F31" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G31" s="3"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>11</v>
       </c>
@@ -1820,11 +1878,12 @@
       <c r="E32" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F32" s="5" t="b">
+      <c r="F32" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G32" s="3"/>
-      <c r="H32" s="1"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
@@ -1840,11 +1899,12 @@
       <c r="E33" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="5" t="b">
+      <c r="F33" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G33" s="3"/>
-      <c r="H33" s="1"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
@@ -1860,11 +1920,12 @@
       <c r="E34" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F34" s="5" t="b">
+      <c r="F34" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G34" s="3"/>
-      <c r="H34" s="1"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
@@ -1878,13 +1939,14 @@
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="5" t="b">
+        <v>66</v>
+      </c>
+      <c r="F35" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G35" s="3"/>
-      <c r="H35" s="1"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
@@ -1900,11 +1962,12 @@
       <c r="E36" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="5" t="b">
+      <c r="F36" s="3" t="b">
         <v>1</v>
       </c>
       <c r="G36" s="3"/>
-      <c r="H36" s="1"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
@@ -1920,11 +1983,12 @@
       <c r="E37" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F37" s="5" t="b">
+      <c r="F37" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G37" s="3"/>
-      <c r="H37" s="1"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
@@ -1940,13 +2004,16 @@
       <c r="E38" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="5" t="b">
+      <c r="F38" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="1"/>
+      <c r="H38" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I38" s="3"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
@@ -1962,11 +2029,12 @@
       <c r="E39" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F39" s="5" t="b">
+      <c r="F39" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G39" s="3"/>
-      <c r="H39" s="1"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
@@ -1982,13 +2050,16 @@
       <c r="E40" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F40" s="5" t="b">
+      <c r="F40" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H40" s="1"/>
+      <c r="H40" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I40" s="3"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
@@ -2004,11 +2075,12 @@
       <c r="E41" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F41" s="5" t="b">
+      <c r="F41" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G41" s="3"/>
-      <c r="H41" s="1"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
@@ -2024,11 +2096,12 @@
       <c r="E42" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F42" s="5" t="b">
+      <c r="F42" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G42" s="3"/>
-      <c r="H42" s="1"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
@@ -2044,11 +2117,12 @@
       <c r="E43" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F43" s="5" t="b">
+      <c r="F43" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G43" s="3"/>
-      <c r="H43" s="1"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
@@ -2057,19 +2131,19 @@
       <c r="B44" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6" t="s">
+      <c r="D44" s="3"/>
+      <c r="E44" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F44" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G44" s="6"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="9"/>
+      <c r="F44" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
@@ -2078,21 +2152,23 @@
       <c r="B45" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F45" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G45" s="6" t="s">
+      <c r="D45" s="3"/>
+      <c r="E45" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F45" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H45" s="8"/>
-      <c r="I45" s="9"/>
+      <c r="H45" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I45" s="3"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
@@ -2101,19 +2177,19 @@
       <c r="B46" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F46" s="7" t="b">
+      <c r="D46" s="3"/>
+      <c r="E46" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F46" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="9"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
@@ -2122,19 +2198,19 @@
       <c r="B47" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F47" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="9"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
@@ -2143,19 +2219,19 @@
       <c r="B48" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6" t="s">
+      <c r="D48" s="3"/>
+      <c r="E48" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F48" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="9"/>
+      <c r="F48" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
@@ -2164,19 +2240,19 @@
       <c r="B49" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F49" s="7" t="b">
+      <c r="D49" s="3"/>
+      <c r="E49" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F49" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
@@ -2185,19 +2261,19 @@
       <c r="B50" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F50" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F50" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
@@ -2206,23 +2282,23 @@
       <c r="B51" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F51" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G51" s="6" t="s">
+      <c r="D51" s="3"/>
+      <c r="E51" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F51" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H51" s="6" t="s">
+      <c r="H51" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I51" s="6"/>
+      <c r="I51" s="3"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
@@ -2231,23 +2307,23 @@
       <c r="B52" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D52" s="10"/>
-      <c r="E52" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F52" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G52" s="6" t="s">
+      <c r="D52" s="2"/>
+      <c r="E52" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F52" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H52" s="6" t="s">
+      <c r="H52" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I52" s="6"/>
+      <c r="I52" s="3"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
@@ -2256,23 +2332,23 @@
       <c r="B53" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D53" s="10"/>
-      <c r="E53" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F53" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G53" s="6" t="s">
+      <c r="D53" s="2"/>
+      <c r="E53" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G53" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H53" s="6" t="s">
+      <c r="H53" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I53" s="6"/>
+      <c r="I53" s="3"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
@@ -2281,23 +2357,23 @@
       <c r="B54" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D54" s="10"/>
-      <c r="E54" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F54" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G54" s="6" t="s">
+      <c r="D54" s="2"/>
+      <c r="E54" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G54" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H54" s="6" t="s">
+      <c r="H54" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I54" s="6"/>
+      <c r="I54" s="3"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
@@ -2306,19 +2382,19 @@
       <c r="B55" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D55" s="10"/>
-      <c r="E55" s="6" t="s">
+      <c r="D55" s="2"/>
+      <c r="E55" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F55" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
-      <c r="I55" s="6"/>
+      <c r="F55" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
@@ -2327,19 +2403,19 @@
       <c r="B56" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D56" s="10"/>
-      <c r="E56" s="6" t="s">
+      <c r="D56" s="2"/>
+      <c r="E56" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F56" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="6"/>
+      <c r="F56" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
@@ -2348,19 +2424,19 @@
       <c r="B57" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D57" s="10"/>
-      <c r="E57" s="6" t="s">
+      <c r="D57" s="2"/>
+      <c r="E57" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
-      <c r="I57" s="6"/>
+      <c r="F57" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
@@ -2369,19 +2445,19 @@
       <c r="B58" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D58" s="10"/>
-      <c r="E58" s="6" t="s">
+      <c r="D58" s="2"/>
+      <c r="E58" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F58" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
-      <c r="I58" s="6"/>
+      <c r="F58" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
@@ -2390,23 +2466,23 @@
       <c r="B59" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D59" s="10"/>
-      <c r="E59" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F59" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G59" s="6" t="s">
+      <c r="D59" s="2"/>
+      <c r="E59" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F59" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G59" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H59" s="6" t="s">
+      <c r="H59" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I59" s="6"/>
+      <c r="I59" s="3"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
@@ -2415,23 +2491,23 @@
       <c r="B60" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D60" s="10"/>
-      <c r="E60" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F60" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G60" s="6" t="s">
+      <c r="D60" s="2"/>
+      <c r="E60" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F60" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G60" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H60" s="6" t="s">
+      <c r="H60" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I60" s="6"/>
+      <c r="I60" s="3"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
@@ -2440,19 +2516,19 @@
       <c r="B61" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D61" s="10"/>
-      <c r="E61" s="6" t="s">
+      <c r="D61" s="2"/>
+      <c r="E61" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F61" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G61" s="6"/>
-      <c r="H61" s="6"/>
-      <c r="I61" s="6"/>
+      <c r="F61" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
@@ -2461,19 +2537,19 @@
       <c r="B62" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D62" s="10"/>
-      <c r="E62" s="6" t="s">
+      <c r="D62" s="2"/>
+      <c r="E62" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F62" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G62" s="6"/>
-      <c r="H62" s="6"/>
-      <c r="I62" s="6"/>
+      <c r="F62" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
@@ -2482,23 +2558,23 @@
       <c r="B63" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D63" s="10"/>
-      <c r="E63" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F63" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H63" s="6" t="s">
+      <c r="D63" s="2"/>
+      <c r="E63" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F63" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H63" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I63" s="6"/>
+      <c r="I63" s="3"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
@@ -2507,19 +2583,19 @@
       <c r="B64" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D64" s="10"/>
-      <c r="E64" s="6" t="s">
+      <c r="D64" s="2"/>
+      <c r="E64" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F64" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G64" s="6"/>
-      <c r="H64" s="6"/>
-      <c r="I64" s="6"/>
+      <c r="F64" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
@@ -2528,19 +2604,19 @@
       <c r="B65" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C65" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D65" s="10"/>
-      <c r="E65" s="6" t="s">
+      <c r="D65" s="2"/>
+      <c r="E65" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G65" s="6"/>
-      <c r="H65" s="6"/>
-      <c r="I65" s="6"/>
+      <c r="F65" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
@@ -2549,23 +2625,23 @@
       <c r="B66" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D66" s="10"/>
-      <c r="E66" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F66" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G66" s="6" t="s">
+      <c r="D66" s="2"/>
+      <c r="E66" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F66" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G66" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H66" s="6" t="s">
+      <c r="H66" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I66" s="6"/>
+      <c r="I66" s="3"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
@@ -2574,19 +2650,19 @@
       <c r="B67" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C67" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D67" s="10"/>
-      <c r="E67" s="6" t="s">
+      <c r="D67" s="2"/>
+      <c r="E67" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F67" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G67" s="6"/>
-      <c r="H67" s="6"/>
-      <c r="I67" s="6"/>
+      <c r="F67" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
@@ -2595,23 +2671,23 @@
       <c r="B68" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C68" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F68" s="7" t="b">
+      <c r="D68" s="3"/>
+      <c r="E68" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F68" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="G68" s="6" t="s">
+      <c r="G68" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H68" s="6" t="s">
+      <c r="H68" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I68" s="6"/>
+      <c r="I68" s="3"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
@@ -2620,21 +2696,21 @@
       <c r="B69" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C69" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="D69" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E69" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F69" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G69" s="6"/>
-      <c r="H69" s="6"/>
-      <c r="I69" s="6"/>
+      <c r="E69" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F69" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
@@ -2643,23 +2719,23 @@
       <c r="B70" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C70" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D70" s="6"/>
-      <c r="E70" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F70" s="7" t="b">
+      <c r="D70" s="3"/>
+      <c r="E70" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F70" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="G70" s="6" t="s">
+      <c r="G70" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H70" s="6" t="s">
+      <c r="H70" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I70" s="6"/>
+      <c r="I70" s="3"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
@@ -2668,23 +2744,23 @@
       <c r="B71" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C71" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D71" s="6"/>
-      <c r="E71" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F71" s="7" t="b">
+      <c r="D71" s="3"/>
+      <c r="E71" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F71" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="G71" s="6" t="s">
+      <c r="G71" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H71" s="6" t="s">
+      <c r="H71" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I71" s="6"/>
+      <c r="I71" s="3"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
@@ -2693,21 +2769,21 @@
       <c r="B72" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C72" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D72" s="6" t="s">
+      <c r="D72" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E72" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F72" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G72" s="6"/>
-      <c r="H72" s="9"/>
-      <c r="I72" s="9"/>
+      <c r="E72" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F72" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated the quantity report tables to deconflict from flexfile (remarks)
</commit_message>
<xml_diff>
--- a/data-raw/quantity-tables.xlsx
+++ b/data-raw/quantity-tables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\D78BYMS1\Private\bberkman\My Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajames\Software\Git Local\costverse\readflexfile\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12048" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,6 @@
     <t>SummaryRemark</t>
   </si>
   <si>
-    <t>summaryremarks</t>
-  </si>
-  <si>
     <t>WBS</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>WBSElementRemark</t>
   </si>
   <si>
-    <t>wbselementremarks</t>
-  </si>
-  <si>
     <t>AppropriationTypeEnum</t>
   </si>
   <si>
@@ -487,15 +481,28 @@
   </si>
   <si>
     <t>reportcycleenum</t>
+  </si>
+  <si>
+    <t>summaryremarksqdr</t>
+  </si>
+  <si>
+    <t>wbselementremarksqdr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -537,15 +544,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -828,19 +836,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -854,320 +862,320 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="str">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="6" t="str">
         <f>LOWER(A6)</f>
         <v>quantitiesatcompletion</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="str">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="6" t="str">
         <f>LOWER(A7)</f>
         <v>quantitiestodate</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="str">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="6" t="str">
         <f>LOWER(A8)</f>
         <v>productionsequence</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="B11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C13" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="D13" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C14" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>149</v>
+      <c r="D14" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1175,6 +1183,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1182,61 +1191,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="40.33203125" customWidth="1"/>
-    <col min="3" max="3" width="38.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F2" s="5" t="b">
         <v>0</v>
@@ -1244,19 +1253,19 @@
       <c r="G2" s="3"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F3" s="5" t="b">
         <v>0</v>
@@ -1264,19 +1273,19 @@
       <c r="G3" s="3"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" s="3" t="b">
         <v>0</v>
@@ -1285,44 +1294,44 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F6" s="3" t="b">
         <v>0</v>
@@ -1331,19 +1340,19 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F7" s="3" t="b">
         <v>0</v>
@@ -1352,19 +1361,19 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F8" s="3" t="b">
         <v>0</v>
@@ -1373,19 +1382,19 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F9" s="3" t="b">
         <v>0</v>
@@ -1394,19 +1403,19 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F10" s="3" t="b">
         <v>0</v>
@@ -1415,19 +1424,19 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F11" s="3" t="b">
         <v>0</v>
@@ -1436,19 +1445,19 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F12" s="3" t="b">
         <v>0</v>
@@ -1457,19 +1466,19 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F13" s="3" t="b">
         <v>0</v>
@@ -1478,19 +1487,19 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F14" s="3" t="b">
         <v>0</v>
@@ -1499,19 +1508,19 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F15" s="3" t="b">
         <v>0</v>
@@ -1520,19 +1529,19 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F16" s="3" t="b">
         <v>0</v>
@@ -1541,19 +1550,19 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F17" s="3" t="b">
         <v>0</v>
@@ -1562,19 +1571,19 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F18" s="3" t="b">
         <v>0</v>
@@ -1583,44 +1592,44 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F19" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F20" s="3" t="b">
         <v>0</v>
@@ -1629,19 +1638,19 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F21" s="3" t="b">
         <v>0</v>
@@ -1650,19 +1659,19 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F22" s="3" t="b">
         <v>0</v>
@@ -1671,19 +1680,19 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F23" s="3" t="b">
         <v>0</v>
@@ -1692,19 +1701,19 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F24" s="3" t="b">
         <v>0</v>
@@ -1713,44 +1722,44 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F25" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F26" s="3" t="b">
         <v>0</v>
@@ -1759,19 +1768,19 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F27" s="3" t="b">
         <v>0</v>
@@ -1780,19 +1789,19 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F28" s="3" t="b">
         <v>0</v>
@@ -1801,19 +1810,19 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F29" s="3" t="b">
         <v>0</v>
@@ -1822,19 +1831,19 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F30" s="3" t="b">
         <v>0</v>
@@ -1843,19 +1852,19 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F31" s="3" t="b">
         <v>0</v>
@@ -1864,19 +1873,19 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F32" s="3" t="b">
         <v>0</v>
@@ -1885,19 +1894,19 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F33" s="3" t="b">
         <v>0</v>
@@ -1906,19 +1915,19 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F34" s="3" t="b">
         <v>0</v>
@@ -1927,19 +1936,19 @@
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F35" s="3" t="b">
         <v>0</v>
@@ -1948,19 +1957,19 @@
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F36" s="3" t="b">
         <v>1</v>
@@ -1969,19 +1978,19 @@
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F37" s="3" t="b">
         <v>0</v>
@@ -1990,44 +1999,44 @@
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F38" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F39" s="3" t="b">
         <v>0</v>
@@ -2036,44 +2045,44 @@
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F40" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F41" s="3" t="b">
         <v>0</v>
@@ -2082,19 +2091,19 @@
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F42" s="3" t="b">
         <v>0</v>
@@ -2103,19 +2112,19 @@
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F43" s="3" t="b">
         <v>0</v>
@@ -2124,19 +2133,19 @@
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F44" s="3" t="b">
         <v>0</v>
@@ -2145,44 +2154,44 @@
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F45" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I45" s="3"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F46" s="3" t="b">
         <v>1</v>
@@ -2191,19 +2200,19 @@
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F47" s="3" t="b">
         <v>0</v>
@@ -2212,19 +2221,19 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F48" s="3" t="b">
         <v>0</v>
@@ -2233,19 +2242,19 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F49" s="3" t="b">
         <v>1</v>
@@ -2254,19 +2263,19 @@
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F50" s="3" t="b">
         <v>0</v>
@@ -2275,44 +2284,44 @@
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F51" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I51" s="3"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F52" s="3" t="b">
         <v>1</v>
@@ -2321,23 +2330,23 @@
         <v>8</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I52" s="3"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F53" s="3" t="b">
         <v>1</v>
@@ -2346,48 +2355,48 @@
         <v>5</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I53" s="3"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F54" s="3" t="b">
         <v>1</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I54" s="3"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F55" s="3" t="b">
         <v>0</v>
@@ -2396,19 +2405,19 @@
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F56" s="3" t="b">
         <v>0</v>
@@ -2417,19 +2426,19 @@
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F57" s="3" t="b">
         <v>0</v>
@@ -2438,19 +2447,19 @@
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F58" s="3" t="b">
         <v>0</v>
@@ -2459,19 +2468,19 @@
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F59" s="3" t="b">
         <v>1</v>
@@ -2480,48 +2489,48 @@
         <v>8</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I59" s="3"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F60" s="3" t="b">
         <v>1</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I60" s="3"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>145</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F61" s="3" t="b">
         <v>0</v>
@@ -2530,19 +2539,19 @@
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F62" s="3" t="b">
         <v>0</v>
@@ -2551,19 +2560,19 @@
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F63" s="3" t="b">
         <v>1</v>
@@ -2572,23 +2581,23 @@
         <v>5</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I63" s="3"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F64" s="3" t="b">
         <v>1</v>
@@ -2597,19 +2606,19 @@
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F65" s="3" t="b">
         <v>0</v>
@@ -2618,19 +2627,19 @@
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F66" s="3" t="b">
         <v>0</v>
@@ -2639,23 +2648,23 @@
         <v>8</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I66" s="3"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F67" s="3" t="b">
         <v>0</v>
@@ -2664,19 +2673,19 @@
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F68" s="3" t="b">
         <v>1</v>
@@ -2685,25 +2694,25 @@
         <v>8</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I68" s="3"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F69" s="3" t="b">
         <v>0</v>
@@ -2712,19 +2721,19 @@
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F70" s="3" t="b">
         <v>1</v>
@@ -2733,50 +2742,50 @@
         <v>8</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I70" s="3"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F71" s="3" t="b">
         <v>1</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I71" s="3"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F72" s="3" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
bug fix "data" to "date"
</commit_message>
<xml_diff>
--- a/data-raw/quantity-tables.xlsx
+++ b/data-raw/quantity-tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="155">
   <si>
     <t>table</t>
   </si>
@@ -223,9 +223,6 @@
   </si>
   <si>
     <t>PeriodOfPerformance_EndDate</t>
-  </si>
-  <si>
-    <t>period_of_performance_end_data</t>
   </si>
   <si>
     <t>AppropriationTypeID</t>
@@ -499,9 +496,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -550,15 +554,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -842,7 +847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -867,7 +872,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1000,7 +1005,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>4</v>
@@ -1017,7 +1022,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>4</v>
@@ -1034,10 +1039,10 @@
         <v>20</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E11" s="6" t="b">
         <v>0</v>
@@ -1051,10 +1056,10 @@
         <v>21</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E12" s="6" t="b">
         <v>0</v>
@@ -1068,10 +1073,10 @@
         <v>22</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E13" s="6" t="b">
         <v>0</v>
@@ -1085,10 +1090,10 @@
         <v>23</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E14" s="6" t="b">
         <v>0</v>
@@ -1104,7 +1109,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1145,7 +1152,7 @@
         <v>35</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1153,10 +1160,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>38</v>
@@ -1174,10 +1181,10 @@
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>38</v>
@@ -1195,10 +1202,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>38</v>
@@ -1241,10 +1248,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>38</v>
@@ -1261,10 +1268,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>38</v>
@@ -1281,10 +1288,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>38</v>
@@ -1301,10 +1308,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>38</v>
@@ -1321,10 +1328,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>38</v>
@@ -1341,10 +1348,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>38</v>
@@ -1361,10 +1368,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>38</v>
@@ -1381,10 +1388,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>38</v>
@@ -1401,10 +1408,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>38</v>
@@ -1421,10 +1428,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>38</v>
@@ -1441,10 +1448,10 @@
         <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>38</v>
@@ -1461,10 +1468,10 @@
         <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>38</v>
@@ -1567,10 +1574,10 @@
         <v>11</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>38</v>
@@ -1610,7 +1617,7 @@
         <v>65</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>64</v>
@@ -1627,10 +1634,10 @@
         <v>11</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>38</v>
@@ -1653,10 +1660,10 @@
         <v>11</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>47</v>
@@ -1673,10 +1680,10 @@
         <v>11</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>38</v>
@@ -1693,10 +1700,10 @@
         <v>11</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>49</v>
@@ -1713,10 +1720,10 @@
         <v>11</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>47</v>
@@ -1733,10 +1740,10 @@
         <v>11</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>64</v>
@@ -1753,10 +1760,10 @@
         <v>11</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>38</v>
@@ -1773,10 +1780,10 @@
         <v>11</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>38</v>
@@ -1793,10 +1800,10 @@
         <v>11</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>119</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>38</v>
@@ -1813,10 +1820,10 @@
         <v>11</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>38</v>
@@ -1833,10 +1840,10 @@
         <v>11</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>123</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>64</v>
@@ -2027,8 +2034,8 @@
       <c r="B44" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>66</v>
+      <c r="C44" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>64</v>
@@ -2045,10 +2052,10 @@
         <v>8</v>
       </c>
       <c r="B45" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>38</v>
@@ -2111,10 +2118,10 @@
         <v>15</v>
       </c>
       <c r="B48" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>47</v>
@@ -2171,10 +2178,10 @@
         <v>15</v>
       </c>
       <c r="B51" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>38</v>
@@ -2278,10 +2285,10 @@
         <v>24</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="4" t="s">
@@ -2299,10 +2306,10 @@
         <v>24</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="4" t="s">
@@ -2320,10 +2327,10 @@
         <v>24</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="4" t="s">
@@ -2341,10 +2348,10 @@
         <v>24</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="4" t="s">
@@ -2416,10 +2423,10 @@
         <v>26</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="4" t="s">
@@ -2437,10 +2444,10 @@
         <v>26</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="4" t="s">
@@ -2485,10 +2492,10 @@
         <v>28</v>
       </c>
       <c r="B64" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="4" t="s">
@@ -2506,10 +2513,10 @@
         <v>28</v>
       </c>
       <c r="B65" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="4" t="s">
@@ -2554,10 +2561,10 @@
         <v>28</v>
       </c>
       <c r="B67" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>146</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="4" t="s">
@@ -2607,7 +2614,7 @@
         <v>53</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>38</v>
@@ -2682,7 +2689,7 @@
         <v>53</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>38</v>

</xml_diff>